<commit_message>
Fim do trabalho =)
</commit_message>
<xml_diff>
--- a/Documentos/Casos de teste - Classes de equivalencia.xlsx
+++ b/Documentos/Casos de teste - Classes de equivalencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\UFJF\13º Período\Testes de Software\Trabalhos\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36465DC0-4ADC-4AD8-B2F2-13646BC8693F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D4D3A2-8F33-4B3B-B91B-9A5EE1DE5E51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{DC3EB0D6-1707-4FD3-AD8A-37C0DAA9EE1D}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{DC3EB0D6-1707-4FD3-AD8A-37C0DAA9EE1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Main menu" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Variáveis de entrada</t>
   </si>
@@ -165,6 +165,15 @@
   </si>
   <si>
     <t>I16</t>
+  </si>
+  <si>
+    <t>Menu Principal</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>Start</t>
   </si>
 </sst>
 </file>
@@ -237,12 +246,14 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FBF4D4-F344-4AA3-9F15-9FC13343B7E2}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,104 +586,116 @@
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32424B9C-CD4A-4720-A6DF-A8331335258E}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -681,50 +704,60 @@
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE23AE03-1EFF-4B66-8273-64C5B25D12DE}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,106 +767,116 @@
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>